<commit_message>
Update Geographic Citation Map.xlsx
</commit_message>
<xml_diff>
--- a/assets/Geographic Citation Map.xlsx
+++ b/assets/Geographic Citation Map.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\yin-CV\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91E838DA-096E-4F6E-AE02-F987F05FFDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C46AF1-30D5-429A-A645-C19F1FB335A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="17172" windowWidth="23256" windowHeight="12456" xr2:uid="{3119720D-7FF3-4AFB-8EBC-927CE14F1162}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>China</t>
   </si>
@@ -109,6 +110,15 @@
   </si>
   <si>
     <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Turkey</t>
   </si>
 </sst>
 </file>
@@ -165,7 +175,18 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -476,148 +497,259 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB82C56-AA02-4039-98BD-3183D74C7423}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A4:A29"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
         <v>45430</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1">
+        <v>45453</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="A2:B29">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1572D3B-23DB-4D15-8AA3-926ED30F9F46}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>